<commit_message>
updated master  & ED fig code
</commit_message>
<xml_diff>
--- a/results/source_data/ExtendedDataFigure5_lags.xlsx
+++ b/results/source_data/ExtendedDataFigure5_lags.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="48">
   <si>
     <t>adm0</t>
   </si>
@@ -145,6 +145,21 @@
   <si>
     <t>se</t>
   </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>grp</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
 </sst>
 </file>
 
@@ -1643,13 +1658,13 @@
         <v>8</v>
       </c>
       <c r="C86" s="0">
-        <v>0.109449103474617</v>
+        <v>0.10748159885406494</v>
       </c>
       <c r="D86" s="0">
-        <v>-0.0074080000631511211</v>
+        <v>-0.0033799000084400177</v>
       </c>
       <c r="E86" s="0">
-        <v>0.22630620002746582</v>
+        <v>0.21834300458431244</v>
       </c>
     </row>
     <row r="87">
@@ -1660,13 +1675,13 @@
         <v>8</v>
       </c>
       <c r="C87" s="0">
-        <v>0.11086250096559525</v>
+        <v>0.10447029769420624</v>
       </c>
       <c r="D87" s="0">
-        <v>-0.0043629999272525311</v>
+        <v>-0.0095266001299023628</v>
       </c>
       <c r="E87" s="0">
-        <v>0.22608789801597595</v>
+        <v>0.21846729516983032</v>
       </c>
     </row>
     <row r="88">
@@ -1677,13 +1692,13 @@
         <v>8</v>
       </c>
       <c r="C88" s="0">
-        <v>0.13268910348415375</v>
+        <v>0.12652599811553955</v>
       </c>
       <c r="D88" s="0">
-        <v>0.013171699829399586</v>
+        <v>0.013032699935138226</v>
       </c>
       <c r="E88" s="0">
-        <v>0.25220650434494019</v>
+        <v>0.2400193065404892</v>
       </c>
     </row>
     <row r="89">
@@ -1694,13 +1709,13 @@
         <v>8</v>
       </c>
       <c r="C89" s="0">
-        <v>0.11051350086927414</v>
+        <v>0.10487180203199387</v>
       </c>
       <c r="D89" s="0">
-        <v>-0.046129599213600159</v>
+        <v>-0.045122500509023666</v>
       </c>
       <c r="E89" s="0">
-        <v>0.26715660095214844</v>
+        <v>0.25486600399017334</v>
       </c>
     </row>
     <row r="90">
@@ -1711,13 +1726,13 @@
         <v>8</v>
       </c>
       <c r="C90" s="0">
-        <v>0.10775099694728851</v>
+        <v>0.10629530251026154</v>
       </c>
       <c r="D90" s="0">
-        <v>-0.045602999627590179</v>
+        <v>-0.03134860098361969</v>
       </c>
       <c r="E90" s="0">
-        <v>0.26110509037971497</v>
+        <v>0.24393920600414276</v>
       </c>
     </row>
     <row r="91">
@@ -1728,13 +1743,13 @@
         <v>8</v>
       </c>
       <c r="C91" s="0">
-        <v>0.14393700659275055</v>
+        <v>0.14786510169506073</v>
       </c>
       <c r="D91" s="0">
-        <v>-0.0059678000397980213</v>
+        <v>0.011944499798119068</v>
       </c>
       <c r="E91" s="0">
-        <v>0.2938418984413147</v>
+        <v>0.2837856113910675</v>
       </c>
     </row>
     <row r="92">
@@ -1745,13 +1760,13 @@
         <v>12</v>
       </c>
       <c r="C92" s="0">
-        <v>-0.071544401347637177</v>
+        <v>-0.071390002965927124</v>
       </c>
       <c r="D92" s="0">
-        <v>-0.13756850361824036</v>
+        <v>-0.13743330538272858</v>
       </c>
       <c r="E92" s="0">
-        <v>-0.0055203000083565712</v>
+        <v>-0.0053468002006411552</v>
       </c>
     </row>
     <row r="93">
@@ -1762,13 +1777,13 @@
         <v>12</v>
       </c>
       <c r="C93" s="0">
-        <v>-0.070099897682666779</v>
+        <v>-0.06959100067615509</v>
       </c>
       <c r="D93" s="0">
-        <v>-0.13455469906330109</v>
+        <v>-0.13422690331935883</v>
       </c>
       <c r="E93" s="0">
-        <v>-0.0056451000273227692</v>
+        <v>-0.0049550998955965042</v>
       </c>
     </row>
     <row r="94">
@@ -1779,13 +1794,13 @@
         <v>12</v>
       </c>
       <c r="C94" s="0">
-        <v>-0.089497700333595276</v>
+        <v>-0.089302599430084229</v>
       </c>
       <c r="D94" s="0">
-        <v>-0.16778500378131866</v>
+        <v>-0.16768769919872284</v>
       </c>
       <c r="E94" s="0">
-        <v>-0.011210300028324127</v>
+        <v>-0.010917499661445618</v>
       </c>
     </row>
     <row r="95">
@@ -1796,13 +1811,13 @@
         <v>12</v>
       </c>
       <c r="C95" s="0">
-        <v>-0.081848502159118652</v>
+        <v>-0.082204900681972504</v>
       </c>
       <c r="D95" s="0">
-        <v>-0.18601010739803314</v>
+        <v>-0.18695579469203949</v>
       </c>
       <c r="E95" s="0">
-        <v>0.022313099354505539</v>
+        <v>0.022546000778675079</v>
       </c>
     </row>
     <row r="96">
@@ -1813,13 +1828,13 @@
         <v>12</v>
       </c>
       <c r="C96" s="0">
-        <v>-0.069333799183368683</v>
+        <v>-0.071125298738479614</v>
       </c>
       <c r="D96" s="0">
-        <v>-0.17769299447536469</v>
+        <v>-0.17949619889259338</v>
       </c>
       <c r="E96" s="0">
-        <v>0.039025299251079559</v>
+        <v>0.037245698273181915</v>
       </c>
     </row>
     <row r="97">
@@ -1830,13 +1845,13 @@
         <v>12</v>
       </c>
       <c r="C97" s="0">
-        <v>-0.1044796034693718</v>
+        <v>-0.10619469732046127</v>
       </c>
       <c r="D97" s="0">
-        <v>-0.24667090177536011</v>
+        <v>-0.24804750084877014</v>
       </c>
       <c r="E97" s="0">
-        <v>0.037711698561906815</v>
+        <v>0.03565799817442894</v>
       </c>
     </row>
     <row r="98">
@@ -1847,13 +1862,13 @@
         <v>13</v>
       </c>
       <c r="C98" s="0">
-        <v>-0.091627001762390137</v>
+        <v>-0.097512401640415192</v>
       </c>
       <c r="D98" s="0">
-        <v>-0.27246600389480591</v>
+        <v>-0.27802440524101257</v>
       </c>
       <c r="E98" s="0">
-        <v>0.089212000370025635</v>
+        <v>0.08299960196018219</v>
       </c>
     </row>
     <row r="99">
@@ -1864,13 +1879,13 @@
         <v>13</v>
       </c>
       <c r="C99" s="0">
-        <v>-0.076046198606491089</v>
+        <v>-0.10215400159358978</v>
       </c>
       <c r="D99" s="0">
-        <v>-0.25786331295967102</v>
+        <v>-0.299925297498703</v>
       </c>
       <c r="E99" s="0">
-        <v>0.10577090084552765</v>
+        <v>0.095617197453975677</v>
       </c>
     </row>
     <row r="100">
@@ -1881,13 +1896,13 @@
         <v>13</v>
       </c>
       <c r="C100" s="0">
-        <v>-0.10961449891328812</v>
+        <v>-0.13940109312534332</v>
       </c>
       <c r="D100" s="0">
-        <v>-0.27170878648757935</v>
+        <v>-0.2904546856880188</v>
       </c>
       <c r="E100" s="0">
-        <v>0.052479799836874008</v>
+        <v>0.011652500368654728</v>
       </c>
     </row>
     <row r="101">
@@ -1898,13 +1913,13 @@
         <v>13</v>
       </c>
       <c r="C101" s="0">
-        <v>-0.1787835955619812</v>
+        <v>-0.20831489562988281</v>
       </c>
       <c r="D101" s="0">
-        <v>-0.32672148942947388</v>
+        <v>-0.3420046865940094</v>
       </c>
       <c r="E101" s="0">
-        <v>-0.030845599249005318</v>
+        <v>-0.074625000357627869</v>
       </c>
     </row>
     <row r="102">
@@ -1915,13 +1930,13 @@
         <v>13</v>
       </c>
       <c r="C102" s="0">
-        <v>-0.051041901111602783</v>
+        <v>-0.082911700010299683</v>
       </c>
       <c r="D102" s="0">
-        <v>-0.26378050446510315</v>
+        <v>-0.25029918551445007</v>
       </c>
       <c r="E102" s="0">
-        <v>0.16169680655002594</v>
+        <v>0.084475800395011902</v>
       </c>
     </row>
     <row r="103">
@@ -1932,13 +1947,13 @@
         <v>13</v>
       </c>
       <c r="C103" s="0">
-        <v>-0.29473239183425903</v>
+        <v>-0.30285158753395081</v>
       </c>
       <c r="D103" s="0">
-        <v>-0.62766540050506592</v>
+        <v>-0.60115867853164673</v>
       </c>
       <c r="E103" s="0">
-        <v>0.038200598210096359</v>
+        <v>-0.0045444001443684101</v>
       </c>
     </row>
     <row r="104">
@@ -1949,13 +1964,13 @@
         <v>9</v>
       </c>
       <c r="C104" s="0">
-        <v>-0.035843100398778915</v>
+        <v>-0.033232599496841431</v>
       </c>
       <c r="D104" s="0">
-        <v>-0.10386709868907928</v>
+        <v>-0.082337602972984314</v>
       </c>
       <c r="E104" s="0">
-        <v>0.032180901616811752</v>
+        <v>0.015872400254011154</v>
       </c>
     </row>
     <row r="105">
@@ -1966,13 +1981,13 @@
         <v>9</v>
       </c>
       <c r="C105" s="0">
-        <v>-0.060416799038648605</v>
+        <v>-0.051409400999546051</v>
       </c>
       <c r="D105" s="0">
-        <v>-0.12904289364814758</v>
+        <v>-0.10298120230436325</v>
       </c>
       <c r="E105" s="0">
-        <v>0.0082093998789787292</v>
+        <v>0.00016239999968092889</v>
       </c>
     </row>
     <row r="106">
@@ -1983,13 +1998,13 @@
         <v>9</v>
       </c>
       <c r="C106" s="0">
-        <v>-0.072772100567817688</v>
+        <v>-0.063374698162078857</v>
       </c>
       <c r="D106" s="0">
-        <v>-0.14425820112228394</v>
+        <v>-0.1118977963924408</v>
       </c>
       <c r="E106" s="0">
-        <v>-0.0012859000125899911</v>
+        <v>-0.014851599931716919</v>
       </c>
     </row>
     <row r="107">
@@ -2000,13 +2015,13 @@
         <v>9</v>
       </c>
       <c r="C107" s="0">
-        <v>-0.081241302192211151</v>
+        <v>-0.071840003132820129</v>
       </c>
       <c r="D107" s="0">
-        <v>-0.1645359992980957</v>
+        <v>-0.12544029951095581</v>
       </c>
       <c r="E107" s="0">
-        <v>0.0020534999202936888</v>
+        <v>-0.018239699304103851</v>
       </c>
     </row>
     <row r="108">
@@ -2017,13 +2032,13 @@
         <v>9</v>
       </c>
       <c r="C108" s="0">
-        <v>-0.098123699426651001</v>
+        <v>-0.09329339861869812</v>
       </c>
       <c r="D108" s="0">
-        <v>-0.19590909779071808</v>
+        <v>-0.14893439412117004</v>
       </c>
       <c r="E108" s="0">
-        <v>-0.00033829998574219644</v>
+        <v>-0.037652399390935898</v>
       </c>
     </row>
     <row r="109">
@@ -2034,13 +2049,13 @@
         <v>9</v>
       </c>
       <c r="C109" s="0">
-        <v>-0.072613798081874847</v>
+        <v>-0.075594097375869751</v>
       </c>
       <c r="D109" s="0">
-        <v>-0.18992440402507782</v>
+        <v>-0.17764079570770264</v>
       </c>
       <c r="E109" s="0">
-        <v>0.04469669982790947</v>
+        <v>0.026452699676156044</v>
       </c>
     </row>
     <row r="110">
@@ -2051,13 +2066,13 @@
         <v>14</v>
       </c>
       <c r="C110" s="0">
-        <v>-0.20193339884281158</v>
+        <v>-0.19842860102653503</v>
       </c>
       <c r="D110" s="0">
-        <v>-0.34516221284866333</v>
+        <v>-0.32032018899917603</v>
       </c>
       <c r="E110" s="0">
-        <v>-0.058704599738121033</v>
+        <v>-0.076536998152732849</v>
       </c>
     </row>
     <row r="111">
@@ -2068,13 +2083,13 @@
         <v>14</v>
       </c>
       <c r="C111" s="0">
-        <v>-0.23005120456218719</v>
+        <v>-0.21864299476146698</v>
       </c>
       <c r="D111" s="0">
-        <v>-0.37059500813484192</v>
+        <v>-0.35286828875541687</v>
       </c>
       <c r="E111" s="0">
-        <v>-0.089507296681404114</v>
+        <v>-0.08441770076751709</v>
       </c>
     </row>
     <row r="112">
@@ -2085,13 +2100,13 @@
         <v>14</v>
       </c>
       <c r="C112" s="0">
-        <v>-0.22273789346218109</v>
+        <v>-0.21136459708213806</v>
       </c>
       <c r="D112" s="0">
-        <v>-0.32684141397476196</v>
+        <v>-0.28460720181465149</v>
       </c>
       <c r="E112" s="0">
-        <v>-0.11863440275192261</v>
+        <v>-0.13812209665775299</v>
       </c>
     </row>
     <row r="113">
@@ -2102,13 +2117,13 @@
         <v>14</v>
       </c>
       <c r="C113" s="0">
-        <v>-0.18319480121135712</v>
+        <v>-0.1720225065946579</v>
       </c>
       <c r="D113" s="0">
-        <v>-0.29410499334335327</v>
+        <v>-0.24977929890155792</v>
       </c>
       <c r="E113" s="0">
-        <v>-0.072284601628780365</v>
+        <v>-0.09426560252904892</v>
       </c>
     </row>
     <row r="114">
@@ -2119,13 +2134,13 @@
         <v>14</v>
       </c>
       <c r="C114" s="0">
-        <v>-0.29198819398880005</v>
+        <v>-0.28620550036430359</v>
       </c>
       <c r="D114" s="0">
-        <v>-0.44041529297828674</v>
+        <v>-0.3914732038974762</v>
       </c>
       <c r="E114" s="0">
-        <v>-0.14356109499931335</v>
+        <v>-0.18093790113925934</v>
       </c>
     </row>
     <row r="115">
@@ -2136,13 +2151,13 @@
         <v>14</v>
       </c>
       <c r="C115" s="0">
-        <v>-0.13739140331745148</v>
+        <v>-0.14190979301929474</v>
       </c>
       <c r="D115" s="0">
-        <v>-0.37145590782165527</v>
+        <v>-0.35764870047569275</v>
       </c>
       <c r="E115" s="0">
-        <v>0.096672996878623962</v>
+        <v>0.073829002678394318</v>
       </c>
     </row>
     <row r="116">
@@ -2153,13 +2168,13 @@
         <v>15</v>
       </c>
       <c r="C116" s="0">
-        <v>0.010583300143480301</v>
+        <v>0.0080816000699996948</v>
       </c>
       <c r="D116" s="0">
-        <v>-0.095673799514770508</v>
+        <v>-0.064301900565624237</v>
       </c>
       <c r="E116" s="0">
-        <v>0.11684049665927887</v>
+        <v>0.080465100705623627</v>
       </c>
     </row>
     <row r="117">
@@ -2170,13 +2185,13 @@
         <v>15</v>
       </c>
       <c r="C117" s="0">
-        <v>0.054612200707197189</v>
+        <v>0.049734398722648621</v>
       </c>
       <c r="D117" s="0">
-        <v>-0.059611100703477859</v>
+        <v>-0.031059300526976585</v>
       </c>
       <c r="E117" s="0">
-        <v>0.16883540153503418</v>
+        <v>0.13052810728549957</v>
       </c>
     </row>
     <row r="118">
@@ -2187,13 +2202,13 @@
         <v>15</v>
       </c>
       <c r="C118" s="0">
-        <v>0.072262600064277649</v>
+        <v>0.068941600620746613</v>
       </c>
       <c r="D118" s="0">
-        <v>-0.035487100481987</v>
+        <v>-0.0056623001582920551</v>
       </c>
       <c r="E118" s="0">
-        <v>0.1800123006105423</v>
+        <v>0.14354559779167175</v>
       </c>
     </row>
     <row r="119">
@@ -2204,13 +2219,13 @@
         <v>15</v>
       </c>
       <c r="C119" s="0">
-        <v>0.082327701151371002</v>
+        <v>0.078925102949142456</v>
       </c>
       <c r="D119" s="0">
-        <v>-0.038458298891782761</v>
+        <v>-0.0025190999731421471</v>
       </c>
       <c r="E119" s="0">
-        <v>0.20311379432678223</v>
+        <v>0.1603693962097168</v>
       </c>
     </row>
     <row r="120">
@@ -2221,13 +2236,13 @@
         <v>15</v>
       </c>
       <c r="C120" s="0">
-        <v>0.11464180052280426</v>
+        <v>0.12155299633741379</v>
       </c>
       <c r="D120" s="0">
-        <v>-0.012749100103974342</v>
+        <v>0.042662199586629868</v>
       </c>
       <c r="E120" s="0">
-        <v>0.24203270673751831</v>
+        <v>0.2004438042640686</v>
       </c>
     </row>
     <row r="121">
@@ -2238,13 +2253,13 @@
         <v>15</v>
       </c>
       <c r="C121" s="0">
-        <v>0.058571700006723404</v>
+        <v>0.069351702928543091</v>
       </c>
       <c r="D121" s="0">
-        <v>-0.080266103148460388</v>
+        <v>-0.051713798195123672</v>
       </c>
       <c r="E121" s="0">
-        <v>0.1974094957113266</v>
+        <v>0.1904170960187912</v>
       </c>
     </row>
     <row r="122">
@@ -2967,27 +2982,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G81"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>46</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2">
@@ -2995,319 +3013,1839 @@
         <v>0</v>
       </c>
       <c r="B2" s="0">
-        <v>0.23181934654712677</v>
+        <v>0</v>
       </c>
       <c r="C2" s="0">
-        <v>0.31242671608924866</v>
-      </c>
-      <c r="D2" s="0">
-        <v>0.29714646935462952</v>
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
       </c>
       <c r="E2" s="0">
-        <v>0.30193653702735901</v>
+        <v>1</v>
       </c>
       <c r="F2" s="0">
-        <v>0.280570387840271</v>
+        <v>0</v>
+      </c>
+      <c r="G2" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="0">
-        <v>0.22948598861694336</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0">
-        <v>0.31771978735923767</v>
-      </c>
-      <c r="D3" s="0">
-        <v>0.32686534523963928</v>
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
       </c>
       <c r="E3" s="0">
-        <v>0.30193650722503662</v>
+        <v>1</v>
       </c>
       <c r="F3" s="0">
-        <v>0.29767808318138123</v>
+        <v>0</v>
+      </c>
+      <c r="G3" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" s="0">
-        <v>0.24363245069980621</v>
+        <v>0</v>
       </c>
       <c r="C4" s="0">
-        <v>0.32881000638008118</v>
-      </c>
-      <c r="D4" s="0">
-        <v>0.35002753138542175</v>
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
       </c>
       <c r="E4" s="0">
-        <v>0.29931876063346863</v>
+        <v>1</v>
       </c>
       <c r="F4" s="0">
-        <v>0.30145007371902466</v>
+        <v>0</v>
+      </c>
+      <c r="G4" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" s="0">
-        <v>0.24472054839134216</v>
+        <v>0</v>
       </c>
       <c r="C5" s="0">
-        <v>0.3129630982875824</v>
-      </c>
-      <c r="D5" s="0">
-        <v>0.37457647919654846</v>
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
       </c>
       <c r="E5" s="0">
-        <v>0.30130875110626221</v>
+        <v>1</v>
       </c>
       <c r="F5" s="0">
-        <v>0.31369751691818237</v>
+        <v>0</v>
+      </c>
+      <c r="G5" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B6" s="0">
-        <v>0.24855084717273712</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0">
-        <v>0.30478754639625549</v>
-      </c>
-      <c r="D6" s="0">
-        <v>0.39304912090301514</v>
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
       </c>
       <c r="E6" s="0">
-        <v>0.30647537112236023</v>
+        <v>1</v>
       </c>
       <c r="F6" s="0">
-        <v>0.30930596590042114</v>
+        <v>0</v>
+      </c>
+      <c r="G6" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B7" s="0">
-        <v>0.24014408886432648</v>
+        <v>0</v>
       </c>
       <c r="C7" s="0">
-        <v>0.3075079619884491</v>
-      </c>
-      <c r="D7" s="0">
-        <v>0.38205805420875549</v>
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
       </c>
       <c r="E7" s="0">
-        <v>0.31476083397865295</v>
+        <v>1</v>
       </c>
       <c r="F7" s="0">
-        <v>0.28975671529769897</v>
+        <v>0</v>
+      </c>
+      <c r="G7" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B8" s="0">
-        <v>0.23417806625366211</v>
+        <v>0</v>
       </c>
       <c r="C8" s="0">
-        <v>0.29653763771057129</v>
-      </c>
-      <c r="D8" s="0">
-        <v>0.38279885053634644</v>
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
       </c>
       <c r="E8" s="0">
-        <v>0.30730077624320984</v>
+        <v>1</v>
       </c>
       <c r="F8" s="0">
-        <v>0.2875497043132782</v>
+        <v>0</v>
+      </c>
+      <c r="G8" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B9" s="0">
-        <v>0.24025264382362366</v>
+        <v>0</v>
       </c>
       <c r="C9" s="0">
-        <v>0.27797049283981323</v>
-      </c>
-      <c r="D9" s="0">
-        <v>0.35442245006561279</v>
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
       </c>
       <c r="E9" s="0">
-        <v>0.31566473841667175</v>
+        <v>1</v>
       </c>
       <c r="F9" s="0">
-        <v>0.26751077175140381</v>
+        <v>0</v>
+      </c>
+      <c r="G9" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B10" s="0">
-        <v>0.23550085723400116</v>
+        <v>0</v>
       </c>
       <c r="C10" s="0">
-        <v>0.26366797089576721</v>
-      </c>
-      <c r="D10" s="0">
-        <v>0.31690052151679993</v>
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
       </c>
       <c r="E10" s="0">
-        <v>0.31042590737342834</v>
+        <v>1</v>
       </c>
       <c r="F10" s="0">
-        <v>0.24179553985595703</v>
+        <v>0</v>
+      </c>
+      <c r="G10" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B11" s="0">
-        <v>0.24521960318088531</v>
+        <v>0</v>
       </c>
       <c r="C11" s="0">
-        <v>0.25027880072593689</v>
-      </c>
-      <c r="D11" s="0">
-        <v>0.29959288239479065</v>
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
       </c>
       <c r="E11" s="0">
-        <v>0.31543931365013123</v>
+        <v>1</v>
       </c>
       <c r="F11" s="0">
-        <v>0.22909201681613922</v>
+        <v>0</v>
+      </c>
+      <c r="G11" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B12" s="0">
-        <v>0.23993898928165436</v>
+        <v>0</v>
       </c>
       <c r="C12" s="0">
-        <v>0.23256926238536835</v>
-      </c>
-      <c r="D12" s="0">
-        <v>0.28787511587142944</v>
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
       </c>
       <c r="E12" s="0">
-        <v>0.32376077771186829</v>
+        <v>1</v>
       </c>
       <c r="F12" s="0">
-        <v>0.21540489792823792</v>
+        <v>0</v>
+      </c>
+      <c r="G12" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B13" s="0">
-        <v>0.2358463853597641</v>
+        <v>0</v>
       </c>
       <c r="C13" s="0">
-        <v>0.21780940890312195</v>
-      </c>
-      <c r="D13" s="0">
-        <v>0.27702182531356812</v>
+        <v>0</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
       </c>
       <c r="E13" s="0">
-        <v>0.31622827053070068</v>
+        <v>1</v>
       </c>
       <c r="F13" s="0">
-        <v>0.21216312050819397</v>
+        <v>0</v>
+      </c>
+      <c r="G13" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B14" s="0">
-        <v>0.23439641296863556</v>
+        <v>0</v>
       </c>
       <c r="C14" s="0">
-        <v>0.20482936501502991</v>
-      </c>
-      <c r="D14" s="0">
-        <v>0.26219266653060913</v>
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
       </c>
       <c r="E14" s="0">
-        <v>0.31255805492401123</v>
+        <v>1</v>
       </c>
       <c r="F14" s="0">
-        <v>0.20137989521026611</v>
+        <v>0</v>
+      </c>
+      <c r="G14" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B15" s="0">
-        <v>0.22927215695381165</v>
+        <v>0</v>
       </c>
       <c r="C15" s="0">
-        <v>0.19412219524383545</v>
-      </c>
-      <c r="D15" s="0">
-        <v>0.2598719596862793</v>
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
       </c>
       <c r="E15" s="0">
-        <v>0.3142678439617157</v>
+        <v>1</v>
       </c>
       <c r="F15" s="0">
-        <v>0.18796758353710175</v>
+        <v>0</v>
+      </c>
+      <c r="G15" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B16" s="0">
-        <v>0.2200695127248764</v>
+        <v>0</v>
       </c>
       <c r="C16" s="0">
-        <v>0.18463544547557831</v>
-      </c>
-      <c r="D16" s="0">
-        <v>0.26000010967254639</v>
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
       </c>
       <c r="E16" s="0">
-        <v>0.30907920002937317</v>
+        <v>1</v>
       </c>
       <c r="F16" s="0">
-        <v>0.19035698473453522</v>
+        <v>0</v>
+      </c>
+      <c r="G16" s="0">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B17" s="0">
-        <v>0.21544615924358368</v>
+        <v>0</v>
       </c>
       <c r="C17" s="0">
-        <v>0.17757156491279602</v>
-      </c>
-      <c r="D17" s="0">
-        <v>0.24156822264194489</v>
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>2</v>
       </c>
       <c r="E17" s="0">
-        <v>0.30068597197532654</v>
+        <v>1</v>
       </c>
       <c r="F17" s="0">
+        <v>0</v>
+      </c>
+      <c r="G17" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0">
+        <v>0.34746518731117249</v>
+      </c>
+      <c r="B18" s="0">
+        <v>0.033178601413965225</v>
+      </c>
+      <c r="C18" s="0">
+        <v>0.20000000298023224</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="0">
+        <v>2</v>
+      </c>
+      <c r="F18" s="0">
+        <v>0.41249528527259827</v>
+      </c>
+      <c r="G18" s="0">
+        <v>0.2824350893497467</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>0.37686300277709961</v>
+      </c>
+      <c r="B19" s="0">
+        <v>0.035720501095056534</v>
+      </c>
+      <c r="C19" s="0">
+        <v>1.2000000476837158</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="0">
+        <v>2</v>
+      </c>
+      <c r="F19" s="0">
+        <v>0.44687521457672119</v>
+      </c>
+      <c r="G19" s="0">
+        <v>0.30685079097747803</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
+        <v>0.39690360426902771</v>
+      </c>
+      <c r="B20" s="0">
+        <v>0.043094001710414886</v>
+      </c>
+      <c r="C20" s="0">
+        <v>2.2000000476837158</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="0">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0">
+        <v>0.48136788606643677</v>
+      </c>
+      <c r="G20" s="0">
+        <v>0.31243941187858582</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>0.41696760058403015</v>
+      </c>
+      <c r="B21" s="0">
+        <v>0.039848800748586655</v>
+      </c>
+      <c r="C21" s="0">
+        <v>3.2000000476837158</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="0">
+        <v>2</v>
+      </c>
+      <c r="F21" s="0">
+        <v>0.49507129192352295</v>
+      </c>
+      <c r="G21" s="0">
+        <v>0.33886390924453735</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
+        <v>0.43678310513496399</v>
+      </c>
+      <c r="B22" s="0">
+        <v>0.041010398417711258</v>
+      </c>
+      <c r="C22" s="0">
+        <v>4.1999998092651367</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="0">
+        <v>2</v>
+      </c>
+      <c r="F22" s="0">
+        <v>0.51716351509094238</v>
+      </c>
+      <c r="G22" s="0">
+        <v>0.3564026951789856</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
+        <v>0.42289999127388</v>
+      </c>
+      <c r="B23" s="0">
+        <v>0.040379200130701065</v>
+      </c>
+      <c r="C23" s="0">
+        <v>5.1999998092651367</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="0">
+        <v>2</v>
+      </c>
+      <c r="F23" s="0">
+        <v>0.50204318761825562</v>
+      </c>
+      <c r="G23" s="0">
+        <v>0.34375679492950439</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
+        <v>0.42353799939155579</v>
+      </c>
+      <c r="B24" s="0">
+        <v>0.040392998605966568</v>
+      </c>
+      <c r="C24" s="0">
+        <v>6.1999998092651367</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="0">
+        <v>2</v>
+      </c>
+      <c r="F24" s="0">
+        <v>0.5027083158493042</v>
+      </c>
+      <c r="G24" s="0">
+        <v>0.34436771273612976</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
+        <v>0.39814010262489319</v>
+      </c>
+      <c r="B25" s="0">
+        <v>0.038309801369905472</v>
+      </c>
+      <c r="C25" s="0">
+        <v>7.1999998092651367</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="0">
+        <v>2</v>
+      </c>
+      <c r="F25" s="0">
+        <v>0.47322729229927063</v>
+      </c>
+      <c r="G25" s="0">
+        <v>0.32305291295051575</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>0.36208769679069519</v>
+      </c>
+      <c r="B26" s="0">
+        <v>0.034304298460483551</v>
+      </c>
+      <c r="C26" s="0">
+        <v>8.1999998092651367</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="0">
+        <v>2</v>
+      </c>
+      <c r="F26" s="0">
+        <v>0.42932409048080444</v>
+      </c>
+      <c r="G26" s="0">
+        <v>0.29485130310058594</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
+        <v>0.34748819470405579</v>
+      </c>
+      <c r="B27" s="0">
+        <v>0.034906700253486633</v>
+      </c>
+      <c r="C27" s="0">
+        <v>9.1999998092651367</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="0">
+        <v>2</v>
+      </c>
+      <c r="F27" s="0">
+        <v>0.41590529680252075</v>
+      </c>
+      <c r="G27" s="0">
+        <v>0.27907109260559082</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
+        <v>0.33672469854354858</v>
+      </c>
+      <c r="B28" s="0">
+        <v>0.03242579847574234</v>
+      </c>
+      <c r="C28" s="0">
+        <v>10.199999809265137</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="0">
+        <v>2</v>
+      </c>
+      <c r="F28" s="0">
+        <v>0.40027931332588196</v>
+      </c>
+      <c r="G28" s="0">
+        <v>0.2731701135635376</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
+        <v>0.32296329736709595</v>
+      </c>
+      <c r="B29" s="0">
+        <v>0.03399369865655899</v>
+      </c>
+      <c r="C29" s="0">
+        <v>11.199999809265137</v>
+      </c>
+      <c r="D29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="0">
+        <v>2</v>
+      </c>
+      <c r="F29" s="0">
+        <v>0.38959088921546936</v>
+      </c>
+      <c r="G29" s="0">
+        <v>0.25633558630943298</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0">
+        <v>0.31146660447120667</v>
+      </c>
+      <c r="B30" s="0">
+        <v>0.031351599842309952</v>
+      </c>
+      <c r="C30" s="0">
+        <v>12.199999809265137</v>
+      </c>
+      <c r="D30" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="0">
+        <v>2</v>
+      </c>
+      <c r="F30" s="0">
+        <v>0.37291568517684937</v>
+      </c>
+      <c r="G30" s="0">
+        <v>0.25001749396324158</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0">
+        <v>0.30895420908927917</v>
+      </c>
+      <c r="B31" s="0">
+        <v>0.033208098262548447</v>
+      </c>
+      <c r="C31" s="0">
+        <v>13.199999809265137</v>
+      </c>
+      <c r="D31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="0">
+        <v>2</v>
+      </c>
+      <c r="F31" s="0">
+        <v>0.3740420937538147</v>
+      </c>
+      <c r="G31" s="0">
+        <v>0.24386629462242126</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0">
+        <v>0.30937731266021729</v>
+      </c>
+      <c r="B32" s="0">
+        <v>0.032332498580217361</v>
+      </c>
+      <c r="C32" s="0">
+        <v>14.199999809265137</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="0">
+        <v>2</v>
+      </c>
+      <c r="F32" s="0">
+        <v>0.37274900078773499</v>
+      </c>
+      <c r="G32" s="0">
+        <v>0.2460055947303772</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0">
+        <v>0.29045650362968445</v>
+      </c>
+      <c r="B33" s="0">
+        <v>0.032064501196146011</v>
+      </c>
+      <c r="C33" s="0">
+        <v>15.199999809265137</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="0">
+        <v>2</v>
+      </c>
+      <c r="F33" s="0">
+        <v>0.35330289602279663</v>
+      </c>
+      <c r="G33" s="0">
+        <v>0.22761009633541107</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0">
+        <v>0.280570387840271</v>
+      </c>
+      <c r="B34" s="0">
+        <v>0.061418000608682632</v>
+      </c>
+      <c r="C34" s="0">
+        <v>0.40000000596046448</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="0">
+        <v>4</v>
+      </c>
+      <c r="F34" s="0">
+        <v>0.40094968676567078</v>
+      </c>
+      <c r="G34" s="0">
+        <v>0.16019110381603241</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0">
+        <v>0.29767811298370361</v>
+      </c>
+      <c r="B35" s="0">
+        <v>0.060981899499893188</v>
+      </c>
+      <c r="C35" s="0">
+        <v>1.3999999761581421</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="0">
+        <v>4</v>
+      </c>
+      <c r="F35" s="0">
+        <v>0.41720259189605713</v>
+      </c>
+      <c r="G35" s="0">
+        <v>0.17815360426902771</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0">
+        <v>0.30145010352134705</v>
+      </c>
+      <c r="B36" s="0">
+        <v>0.060592301189899445</v>
+      </c>
+      <c r="C36" s="0">
+        <v>2.4000000953674316</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="0">
+        <v>4</v>
+      </c>
+      <c r="F36" s="0">
+        <v>0.42021098732948303</v>
+      </c>
+      <c r="G36" s="0">
+        <v>0.18268920481204987</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0">
+        <v>0.31369748711585999</v>
+      </c>
+      <c r="B37" s="0">
+        <v>0.056942898780107498</v>
+      </c>
+      <c r="C37" s="0">
+        <v>3.4000000953674316</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="0">
+        <v>4</v>
+      </c>
+      <c r="F37" s="0">
+        <v>0.42530560493469238</v>
+      </c>
+      <c r="G37" s="0">
+        <v>0.20208939909934998</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0">
+        <v>0.30930599570274353</v>
+      </c>
+      <c r="B38" s="0">
+        <v>0.058117099106311798</v>
+      </c>
+      <c r="C38" s="0">
+        <v>4.4000000953674316</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="0">
+        <v>4</v>
+      </c>
+      <c r="F38" s="0">
+        <v>0.42321550846099854</v>
+      </c>
+      <c r="G38" s="0">
+        <v>0.19539649784564972</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0">
+        <v>0.28975668549537659</v>
+      </c>
+      <c r="B39" s="0">
+        <v>0.058439701795578003</v>
+      </c>
+      <c r="C39" s="0">
+        <v>5.4000000953674316</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="0">
+        <v>4</v>
+      </c>
+      <c r="F39" s="0">
+        <v>0.40429851412773132</v>
+      </c>
+      <c r="G39" s="0">
+        <v>0.17521490156650543</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0">
+        <v>0.2875497043132782</v>
+      </c>
+      <c r="B40" s="0">
+        <v>0.059206601232290268</v>
+      </c>
+      <c r="C40" s="0">
+        <v>6.4000000953674316</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="0">
+        <v>4</v>
+      </c>
+      <c r="F40" s="0">
+        <v>0.40359461307525635</v>
+      </c>
+      <c r="G40" s="0">
+        <v>0.17150479555130005</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0">
+        <v>0.2675108015537262</v>
+      </c>
+      <c r="B41" s="0">
+        <v>0.059342101216316223</v>
+      </c>
+      <c r="C41" s="0">
+        <v>7.4000000953674316</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="0">
+        <v>4</v>
+      </c>
+      <c r="F41" s="0">
+        <v>0.38382130861282349</v>
+      </c>
+      <c r="G41" s="0">
+        <v>0.15120029449462891</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0">
+        <v>0.24179549515247345</v>
+      </c>
+      <c r="B42" s="0">
+        <v>0.059508699923753738</v>
+      </c>
+      <c r="C42" s="0">
+        <v>8.3999996185302734</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" s="0">
+        <v>4</v>
+      </c>
+      <c r="F42" s="0">
+        <v>0.3584325909614563</v>
+      </c>
+      <c r="G42" s="0">
+        <v>0.1251583993434906</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0">
+        <v>0.22909200191497803</v>
+      </c>
+      <c r="B43" s="0">
+        <v>0.059599798172712326</v>
+      </c>
+      <c r="C43" s="0">
+        <v>9.3999996185302734</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="0">
+        <v>4</v>
+      </c>
+      <c r="F43" s="0">
+        <v>0.34590759873390198</v>
+      </c>
+      <c r="G43" s="0">
+        <v>0.11227639764547348</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0">
+        <v>0.21540489792823792</v>
+      </c>
+      <c r="B44" s="0">
+        <v>0.059326998889446259</v>
+      </c>
+      <c r="C44" s="0">
+        <v>10.399999618530273</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="0">
+        <v>4</v>
+      </c>
+      <c r="F44" s="0">
+        <v>0.33168581128120422</v>
+      </c>
+      <c r="G44" s="0">
+        <v>0.0991239994764328</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0">
+        <v>0.21216310560703278</v>
+      </c>
+      <c r="B45" s="0">
+        <v>0.057766400277614594</v>
+      </c>
+      <c r="C45" s="0">
+        <v>11.399999618530273</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="0">
+        <v>4</v>
+      </c>
+      <c r="F45" s="0">
+        <v>0.32538521289825439</v>
+      </c>
+      <c r="G45" s="0">
+        <v>0.098940998315811157</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0">
+        <v>0.20137989521026611</v>
+      </c>
+      <c r="B46" s="0">
+        <v>0.058563098311424255</v>
+      </c>
+      <c r="C46" s="0">
+        <v>12.399999618530273</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="0">
+        <v>4</v>
+      </c>
+      <c r="F46" s="0">
+        <v>0.31616359949111938</v>
+      </c>
+      <c r="G46" s="0">
+        <v>0.086596198379993439</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0">
+        <v>0.18796759843826294</v>
+      </c>
+      <c r="B47" s="0">
+        <v>0.058849599212408066</v>
+      </c>
+      <c r="C47" s="0">
+        <v>13.399999618530273</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="0">
+        <v>4</v>
+      </c>
+      <c r="F47" s="0">
+        <v>0.30331280827522278</v>
+      </c>
+      <c r="G47" s="0">
+        <v>0.072622403502464294</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0">
+        <v>0.19035699963569641</v>
+      </c>
+      <c r="B48" s="0">
+        <v>0.057244900614023209</v>
+      </c>
+      <c r="C48" s="0">
+        <v>14.399999618530273</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="0">
+        <v>4</v>
+      </c>
+      <c r="F48" s="0">
+        <v>0.30255699157714844</v>
+      </c>
+      <c r="G48" s="0">
+        <v>0.078157000243663788</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0">
         <v>0.17919610440731049</v>
+      </c>
+      <c r="B49" s="0">
+        <v>0.057498998939990997</v>
+      </c>
+      <c r="C49" s="0">
+        <v>15.399999618530273</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="0">
+        <v>4</v>
+      </c>
+      <c r="F49" s="0">
+        <v>0.29189410805702209</v>
+      </c>
+      <c r="G49" s="0">
+        <v>0.066498100757598877</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0">
+        <v>0.29338321089744568</v>
+      </c>
+      <c r="B50" s="0">
+        <v>0.017437299713492393</v>
+      </c>
+      <c r="C50" s="0">
+        <v>0.30000001192092896</v>
+      </c>
+      <c r="D50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="0">
+        <v>3</v>
+      </c>
+      <c r="F50" s="0">
+        <v>0.32756030559539795</v>
+      </c>
+      <c r="G50" s="0">
+        <v>0.25920608639717102</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0">
+        <v>0.29508820176124573</v>
+      </c>
+      <c r="B51" s="0">
+        <v>0.017891800031065941</v>
+      </c>
+      <c r="C51" s="0">
+        <v>1.2999999523162842</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="0">
+        <v>3</v>
+      </c>
+      <c r="F51" s="0">
+        <v>0.33015608787536621</v>
+      </c>
+      <c r="G51" s="0">
+        <v>0.26002028584480286</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>0.28986001014709473</v>
+      </c>
+      <c r="B52" s="0">
+        <v>0.017760999500751495</v>
+      </c>
+      <c r="C52" s="0">
+        <v>2.2999999523162842</v>
+      </c>
+      <c r="D52" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="0">
+        <v>3</v>
+      </c>
+      <c r="F52" s="0">
+        <v>0.32467159628868103</v>
+      </c>
+      <c r="G52" s="0">
+        <v>0.25504851341247559</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>0.29024788737297058</v>
+      </c>
+      <c r="B53" s="0">
+        <v>0.017896700650453568</v>
+      </c>
+      <c r="C53" s="0">
+        <v>3.2999999523162842</v>
+      </c>
+      <c r="D53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" s="0">
+        <v>3</v>
+      </c>
+      <c r="F53" s="0">
+        <v>0.32532539963722229</v>
+      </c>
+      <c r="G53" s="0">
+        <v>0.25517028570175171</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>0.29513809084892273</v>
+      </c>
+      <c r="B54" s="0">
+        <v>0.018136100843548775</v>
+      </c>
+      <c r="C54" s="0">
+        <v>4.3000001907348633</v>
+      </c>
+      <c r="D54" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="0">
+        <v>3</v>
+      </c>
+      <c r="F54" s="0">
+        <v>0.33068481087684631</v>
+      </c>
+      <c r="G54" s="0">
+        <v>0.25959131121635437</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>0.29979559779167175</v>
+      </c>
+      <c r="B55" s="0">
+        <v>0.018005400896072388</v>
+      </c>
+      <c r="C55" s="0">
+        <v>5.3000001907348633</v>
+      </c>
+      <c r="D55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" s="0">
+        <v>3</v>
+      </c>
+      <c r="F55" s="0">
+        <v>0.33508619666099548</v>
+      </c>
+      <c r="G55" s="0">
+        <v>0.26450499892234802</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>0.29152089357376099</v>
+      </c>
+      <c r="B56" s="0">
+        <v>0.018393600359559059</v>
+      </c>
+      <c r="C56" s="0">
+        <v>6.3000001907348633</v>
+      </c>
+      <c r="D56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="0">
+        <v>3</v>
+      </c>
+      <c r="F56" s="0">
+        <v>0.3275722861289978</v>
+      </c>
+      <c r="G56" s="0">
+        <v>0.25546941161155701</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>0.2974143922328949</v>
+      </c>
+      <c r="B57" s="0">
+        <v>0.01839509978890419</v>
+      </c>
+      <c r="C57" s="0">
+        <v>7.3000001907348633</v>
+      </c>
+      <c r="D57" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="0">
+        <v>3</v>
+      </c>
+      <c r="F57" s="0">
+        <v>0.33346879482269287</v>
+      </c>
+      <c r="G57" s="0">
+        <v>0.26135998964309692</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0">
+        <v>0.29235830903053284</v>
+      </c>
+      <c r="B58" s="0">
+        <v>0.018755000084638596</v>
+      </c>
+      <c r="C58" s="0">
+        <v>8.3000001907348633</v>
+      </c>
+      <c r="D58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" s="0">
+        <v>3</v>
+      </c>
+      <c r="F58" s="0">
+        <v>0.32911810278892517</v>
+      </c>
+      <c r="G58" s="0">
+        <v>0.25559848546981812</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0">
+        <v>0.29774799942970276</v>
+      </c>
+      <c r="B59" s="0">
+        <v>0.018401399254798889</v>
+      </c>
+      <c r="C59" s="0">
+        <v>9.3000001907348633</v>
+      </c>
+      <c r="D59" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" s="0">
+        <v>3</v>
+      </c>
+      <c r="F59" s="0">
+        <v>0.33381471037864685</v>
+      </c>
+      <c r="G59" s="0">
+        <v>0.26168128848075867</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0">
+        <v>0.30706891417503357</v>
+      </c>
+      <c r="B60" s="0">
+        <v>0.016943000257015228</v>
+      </c>
+      <c r="C60" s="0">
+        <v>10.300000190734863</v>
+      </c>
+      <c r="D60" t="s">
+        <v>4</v>
+      </c>
+      <c r="E60" s="0">
+        <v>3</v>
+      </c>
+      <c r="F60" s="0">
+        <v>0.34027719497680664</v>
+      </c>
+      <c r="G60" s="0">
+        <v>0.27386060357093811</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0">
+        <v>0.30129900574684143</v>
+      </c>
+      <c r="B61" s="0">
+        <v>0.01647149957716465</v>
+      </c>
+      <c r="C61" s="0">
+        <v>11.300000190734863</v>
+      </c>
+      <c r="D61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="0">
+        <v>3</v>
+      </c>
+      <c r="F61" s="0">
+        <v>0.33358308672904968</v>
+      </c>
+      <c r="G61" s="0">
+        <v>0.26901489496231079</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0">
+        <v>0.2949163019657135</v>
+      </c>
+      <c r="B62" s="0">
+        <v>0.016923399642109871</v>
+      </c>
+      <c r="C62" s="0">
+        <v>12.300000190734863</v>
+      </c>
+      <c r="D62" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="0">
+        <v>3</v>
+      </c>
+      <c r="F62" s="0">
+        <v>0.32808619737625122</v>
+      </c>
+      <c r="G62" s="0">
+        <v>0.26174640655517578</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0">
+        <v>0.29777848720550537</v>
+      </c>
+      <c r="B63" s="0">
+        <v>0.01664000004529953</v>
+      </c>
+      <c r="C63" s="0">
+        <v>13.300000190734863</v>
+      </c>
+      <c r="D63" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="0">
+        <v>3</v>
+      </c>
+      <c r="F63" s="0">
+        <v>0.33039289712905884</v>
+      </c>
+      <c r="G63" s="0">
+        <v>0.26516410708427429</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0">
+        <v>0.29214221239089966</v>
+      </c>
+      <c r="B64" s="0">
+        <v>0.016593899577856064</v>
+      </c>
+      <c r="C64" s="0">
+        <v>14.300000190734863</v>
+      </c>
+      <c r="D64" t="s">
+        <v>4</v>
+      </c>
+      <c r="E64" s="0">
+        <v>3</v>
+      </c>
+      <c r="F64" s="0">
+        <v>0.32466629147529602</v>
+      </c>
+      <c r="G64" s="0">
+        <v>0.25961819291114807</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0">
+        <v>0.28459128737449646</v>
+      </c>
+      <c r="B65" s="0">
+        <v>0.016838500276207924</v>
+      </c>
+      <c r="C65" s="0">
+        <v>15.300000190734863</v>
+      </c>
+      <c r="D65" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="0">
+        <v>3</v>
+      </c>
+      <c r="F65" s="0">
+        <v>0.31759470701217651</v>
+      </c>
+      <c r="G65" s="0">
+        <v>0.25158780813217163</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0">
+        <v>0.32099738717079163</v>
+      </c>
+      <c r="B66" s="0">
+        <v>0.022347800433635712</v>
+      </c>
+      <c r="C66" s="0">
+        <v>0.5</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E66" s="0">
+        <v>5</v>
+      </c>
+      <c r="F66" s="0">
+        <v>0.36479911208152771</v>
+      </c>
+      <c r="G66" s="0">
+        <v>0.27719569206237793</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0">
+        <v>0.31795820593833923</v>
+      </c>
+      <c r="B67" s="0">
+        <v>0.022268999367952347</v>
+      </c>
+      <c r="C67" s="0">
+        <v>1.5</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1</v>
+      </c>
+      <c r="E67" s="0">
+        <v>5</v>
+      </c>
+      <c r="F67" s="0">
+        <v>0.36160540580749512</v>
+      </c>
+      <c r="G67" s="0">
+        <v>0.27431100606918335</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0">
+        <v>0.32458770275115967</v>
+      </c>
+      <c r="B68" s="0">
+        <v>0.023173099383711815</v>
+      </c>
+      <c r="C68" s="0">
+        <v>2.5</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1</v>
+      </c>
+      <c r="E68" s="0">
+        <v>5</v>
+      </c>
+      <c r="F68" s="0">
+        <v>0.37000700831413269</v>
+      </c>
+      <c r="G68" s="0">
+        <v>0.27916839718818665</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0">
+        <v>0.32443758845329285</v>
+      </c>
+      <c r="B69" s="0">
+        <v>0.022644000127911568</v>
+      </c>
+      <c r="C69" s="0">
+        <v>3.5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" s="0">
+        <v>5</v>
+      </c>
+      <c r="F69" s="0">
+        <v>0.36881980299949646</v>
+      </c>
+      <c r="G69" s="0">
+        <v>0.28005531430244446</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0">
+        <v>0.32579758763313293</v>
+      </c>
+      <c r="B70" s="0">
+        <v>0.022622900083661079</v>
+      </c>
+      <c r="C70" s="0">
+        <v>4.5</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1</v>
+      </c>
+      <c r="E70" s="0">
+        <v>5</v>
+      </c>
+      <c r="F70" s="0">
+        <v>0.3701384961605072</v>
+      </c>
+      <c r="G70" s="0">
+        <v>0.28145670890808105</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0">
+        <v>0.32634431123733521</v>
+      </c>
+      <c r="B71" s="0">
+        <v>0.021670600399374962</v>
+      </c>
+      <c r="C71" s="0">
+        <v>5.5</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1</v>
+      </c>
+      <c r="E71" s="0">
+        <v>5</v>
+      </c>
+      <c r="F71" s="0">
+        <v>0.36881870031356812</v>
+      </c>
+      <c r="G71" s="0">
+        <v>0.28386989235877991</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0">
+        <v>0.31835758686065674</v>
+      </c>
+      <c r="B72" s="0">
+        <v>0.021448599174618721</v>
+      </c>
+      <c r="C72" s="0">
+        <v>6.5</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1</v>
+      </c>
+      <c r="E72" s="0">
+        <v>5</v>
+      </c>
+      <c r="F72" s="0">
+        <v>0.36039680242538452</v>
+      </c>
+      <c r="G72" s="0">
+        <v>0.27631831169128418</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="0">
+        <v>0.32959121465682983</v>
+      </c>
+      <c r="B73" s="0">
+        <v>0.021371699869632721</v>
+      </c>
+      <c r="C73" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73" s="0">
+        <v>5</v>
+      </c>
+      <c r="F73" s="0">
+        <v>0.37147969007492065</v>
+      </c>
+      <c r="G73" s="0">
+        <v>0.28770270943641663</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="0">
+        <v>0.32659938931465149</v>
+      </c>
+      <c r="B74" s="0">
+        <v>0.021072300150990486</v>
+      </c>
+      <c r="C74" s="0">
+        <v>8.5</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" s="0">
+        <v>5</v>
+      </c>
+      <c r="F74" s="0">
+        <v>0.36790108680725098</v>
+      </c>
+      <c r="G74" s="0">
+        <v>0.285297691822052</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="0">
+        <v>0.33198699355125427</v>
+      </c>
+      <c r="B75" s="0">
+        <v>0.021804699674248695</v>
+      </c>
+      <c r="C75" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1</v>
+      </c>
+      <c r="E75" s="0">
+        <v>5</v>
+      </c>
+      <c r="F75" s="0">
+        <v>0.37472420930862427</v>
+      </c>
+      <c r="G75" s="0">
+        <v>0.28924980759620667</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="0">
+        <v>0.32885530591011047</v>
+      </c>
+      <c r="B76" s="0">
+        <v>0.020213000476360321</v>
+      </c>
+      <c r="C76" s="0">
+        <v>10.5</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1</v>
+      </c>
+      <c r="E76" s="0">
+        <v>5</v>
+      </c>
+      <c r="F76" s="0">
+        <v>0.36847281455993652</v>
+      </c>
+      <c r="G76" s="0">
+        <v>0.28923779726028442</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="0">
+        <v>0.32469359040260315</v>
+      </c>
+      <c r="B77" s="0">
+        <v>0.019905600696802139</v>
+      </c>
+      <c r="C77" s="0">
+        <v>11.5</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1</v>
+      </c>
+      <c r="E77" s="0">
+        <v>5</v>
+      </c>
+      <c r="F77" s="0">
+        <v>0.36370858550071716</v>
+      </c>
+      <c r="G77" s="0">
+        <v>0.28567859530448914</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="0">
+        <v>0.3218575119972229</v>
+      </c>
+      <c r="B78" s="0">
+        <v>0.018580600619316101</v>
+      </c>
+      <c r="C78" s="0">
+        <v>12.5</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1</v>
+      </c>
+      <c r="E78" s="0">
+        <v>5</v>
+      </c>
+      <c r="F78" s="0">
+        <v>0.35827550292015076</v>
+      </c>
+      <c r="G78" s="0">
+        <v>0.28543949127197266</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="0">
+        <v>0.3150830864906311</v>
+      </c>
+      <c r="B79" s="0">
+        <v>0.019055500626564026</v>
+      </c>
+      <c r="C79" s="0">
+        <v>13.5</v>
+      </c>
+      <c r="D79" t="s">
+        <v>1</v>
+      </c>
+      <c r="E79" s="0">
+        <v>5</v>
+      </c>
+      <c r="F79" s="0">
+        <v>0.35243189334869385</v>
+      </c>
+      <c r="G79" s="0">
+        <v>0.27773430943489075</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="0">
+        <v>0.30781561136245728</v>
+      </c>
+      <c r="B80" s="0">
+        <v>0.018952900543808937</v>
+      </c>
+      <c r="C80" s="0">
+        <v>14.5</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1</v>
+      </c>
+      <c r="E80" s="0">
+        <v>5</v>
+      </c>
+      <c r="F80" s="0">
+        <v>0.34496331214904785</v>
+      </c>
+      <c r="G80" s="0">
+        <v>0.2706679105758667</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="0">
+        <v>0.3023642897605896</v>
+      </c>
+      <c r="B81" s="0">
+        <v>0.018754100427031517</v>
+      </c>
+      <c r="C81" s="0">
+        <v>15.5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1</v>
+      </c>
+      <c r="E81" s="0">
+        <v>5</v>
+      </c>
+      <c r="F81" s="0">
+        <v>0.33912229537963867</v>
+      </c>
+      <c r="G81" s="0">
+        <v>0.26560631394386292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>